<commit_message>
JLCPCB assembly notes added to components information
</commit_message>
<xml_diff>
--- a/PCB and BOM/IMPORTANT_components_information.xlsx
+++ b/PCB and BOM/IMPORTANT_components_information.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="110">
   <si>
     <t>74HC595</t>
   </si>
@@ -342,7 +342,13 @@
     <t>https://www.aliexpress.com/item/32797618620.html?spm=a2g0s.9042311.0.0.27424c4dcRtysh</t>
   </si>
   <si>
-    <t>Please note that some of the components are not available for JLCPCB assembly. You will have to order those separatery and solder them yourself. Everything can be ordered from LCSC.</t>
+    <t>1) Please note that some of the components are not available for JLCPCB assembly. You will have to order those separatery and solder them yourself. Everything can be ordered from LCSC.</t>
+  </si>
+  <si>
+    <t>2) If you order JLCPCB assembly, make sure they position display LEDs with cathodes pointing to bottom left as it's not obvious from the silk screen.</t>
+  </si>
+  <si>
+    <t>IMPORTANT ASSEMBLY NOTES:</t>
   </si>
 </sst>
 </file>
@@ -755,10 +761,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:H83"/>
+  <dimension ref="B2:H83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -771,6 +777,11 @@
     <col min="8" max="8" width="193.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="2:8">
+      <c r="B2" t="s">
+        <v>109</v>
+      </c>
+    </row>
     <row r="3" spans="2:8" ht="15">
       <c r="B3" s="8" t="s">
         <v>107</v>
@@ -782,6 +793,17 @@
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
     </row>
+    <row r="4" spans="2:8" ht="15">
+      <c r="B4" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+    </row>
     <row r="6" spans="2:8">
       <c r="B6" s="4" t="s">
         <v>13</v>
@@ -1515,8 +1537,9 @@
       <c r="C83" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B4:H4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H26" r:id="rId1"/>

</xml_diff>